<commit_message>
MainBoard: Fix pinout.xlsx and STM32F103VCTx.ioc
</commit_message>
<xml_diff>
--- a/hw/pinout.xlsx
+++ b/hw/pinout.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\RB3204-RBCX\ele\MainBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\RB3204-RBCX\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CC2F07-2096-4EC7-B468-F7AF9F567D33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870510B9-F3CC-4D8C-8782-98F6221F6DE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{08978B24-E42F-429B-A3F9-EF8F7AA6C2ED}"/>
   </bookViews>
@@ -2484,57 +2484,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2559,12 +2508,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2906,8 +2906,8 @@
   <dimension ref="A1:AV114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AU10" sqref="AU10"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AU93" sqref="AU93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2936,90 +2936,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="143" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="122" t="s">
+      <c r="B1" s="146" t="s">
         <v>259</v>
       </c>
       <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="132" t="s">
+      <c r="D1" s="139" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="134"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="132" t="s">
+      <c r="E1" s="140"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="139" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="133"/>
-      <c r="K1" s="132" t="s">
+      <c r="H1" s="140"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="139" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="133"/>
-      <c r="N1" s="132" t="s">
+      <c r="L1" s="140"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="139" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="133"/>
-      <c r="P1" s="126" t="s">
+      <c r="O1" s="141"/>
+      <c r="P1" s="129" t="s">
         <v>94</v>
       </c>
-      <c r="Q1" s="126" t="s">
+      <c r="Q1" s="129" t="s">
         <v>95</v>
       </c>
-      <c r="R1" s="128" t="s">
+      <c r="R1" s="131" t="s">
         <v>115</v>
       </c>
-      <c r="S1" s="129"/>
-      <c r="T1" s="128" t="s">
+      <c r="S1" s="132"/>
+      <c r="T1" s="131" t="s">
         <v>113</v>
       </c>
-      <c r="U1" s="129"/>
-      <c r="V1" s="132" t="s">
+      <c r="U1" s="132"/>
+      <c r="V1" s="139" t="s">
         <v>116</v>
       </c>
-      <c r="W1" s="134"/>
-      <c r="X1" s="133"/>
-      <c r="Y1" s="126" t="s">
+      <c r="W1" s="140"/>
+      <c r="X1" s="141"/>
+      <c r="Y1" s="129" t="s">
         <v>305</v>
       </c>
-      <c r="Z1" s="126" t="s">
+      <c r="Z1" s="129" t="s">
         <v>306</v>
       </c>
-      <c r="AA1" s="128" t="s">
+      <c r="AA1" s="131" t="s">
         <v>123</v>
       </c>
-      <c r="AB1" s="137"/>
-      <c r="AC1" s="129"/>
-      <c r="AD1" s="128" t="s">
+      <c r="AB1" s="142"/>
+      <c r="AC1" s="132"/>
+      <c r="AD1" s="131" t="s">
         <v>124</v>
       </c>
-      <c r="AE1" s="129"/>
+      <c r="AE1" s="132"/>
       <c r="AF1" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="AG1" s="138" t="s">
+      <c r="AG1" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="AH1" s="139"/>
-      <c r="AI1" s="135" t="s">
+      <c r="AH1" s="134"/>
+      <c r="AI1" s="137" t="s">
         <v>126</v>
       </c>
-      <c r="AJ1" s="138" t="s">
+      <c r="AJ1" s="133" t="s">
         <v>127</v>
       </c>
-      <c r="AK1" s="139"/>
-      <c r="AL1" s="126" t="s">
+      <c r="AK1" s="134"/>
+      <c r="AL1" s="129" t="s">
         <v>129</v>
       </c>
-      <c r="AM1" s="148" t="s">
+      <c r="AM1" s="135" t="s">
         <v>130</v>
       </c>
-      <c r="AN1" s="135" t="s">
+      <c r="AN1" s="137" t="s">
         <v>151</v>
       </c>
       <c r="AO1" s="8" t="s">
@@ -3034,22 +3034,22 @@
       <c r="AR1" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="AS1" s="140" t="s">
+      <c r="AS1" s="121" t="s">
         <v>141</v>
       </c>
-      <c r="AT1" s="142" t="s">
+      <c r="AT1" s="123" t="s">
         <v>182</v>
       </c>
-      <c r="AU1" s="144" t="s">
+      <c r="AU1" s="125" t="s">
         <v>183</v>
       </c>
-      <c r="AV1" s="146" t="s">
+      <c r="AV1" s="127" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="131"/>
-      <c r="B2" s="123"/>
+      <c r="A2" s="144"/>
+      <c r="B2" s="147"/>
       <c r="C2" s="37" t="s">
         <v>96</v>
       </c>
@@ -3089,8 +3089,8 @@
       <c r="O2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="127"/>
-      <c r="Q2" s="127"/>
+      <c r="P2" s="130"/>
+      <c r="Q2" s="130"/>
       <c r="R2" s="9" t="s">
         <v>105</v>
       </c>
@@ -3112,8 +3112,8 @@
       <c r="X2" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="Y2" s="127"/>
-      <c r="Z2" s="127"/>
+      <c r="Y2" s="130"/>
+      <c r="Z2" s="130"/>
       <c r="AA2" s="9" t="s">
         <v>101</v>
       </c>
@@ -3136,24 +3136,24 @@
       <c r="AH2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="AI2" s="136"/>
+      <c r="AI2" s="138"/>
       <c r="AJ2" s="9" t="s">
         <v>105</v>
       </c>
       <c r="AK2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="AL2" s="127"/>
-      <c r="AM2" s="149"/>
-      <c r="AN2" s="136"/>
+      <c r="AL2" s="130"/>
+      <c r="AM2" s="136"/>
+      <c r="AN2" s="138"/>
       <c r="AO2" s="16"/>
       <c r="AP2" s="16"/>
       <c r="AQ2" s="16"/>
       <c r="AR2" s="16"/>
-      <c r="AS2" s="141"/>
-      <c r="AT2" s="143"/>
-      <c r="AU2" s="145"/>
-      <c r="AV2" s="147"/>
+      <c r="AS2" s="122"/>
+      <c r="AT2" s="124"/>
+      <c r="AU2" s="126"/>
+      <c r="AV2" s="128"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="74">
@@ -5588,7 +5588,7 @@
         <v>108</v>
       </c>
       <c r="AU41" s="29" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AV41" s="28"/>
     </row>
@@ -5648,7 +5648,7 @@
         <v>97</v>
       </c>
       <c r="AU42" s="29" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AV42" s="28"/>
     </row>
@@ -5708,7 +5708,7 @@
         <v>110</v>
       </c>
       <c r="AU43" s="29" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AV43" s="28"/>
     </row>
@@ -5768,7 +5768,7 @@
         <v>98</v>
       </c>
       <c r="AU44" s="29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AV44" s="28"/>
     </row>
@@ -5828,7 +5828,7 @@
         <v>111</v>
       </c>
       <c r="AU45" s="29" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AV45" s="28"/>
     </row>
@@ -5888,7 +5888,7 @@
         <v>99</v>
       </c>
       <c r="AU46" s="29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AV46" s="28"/>
     </row>
@@ -9398,70 +9398,70 @@
       </c>
       <c r="B103" s="30"/>
       <c r="C103" s="30"/>
-      <c r="D103" s="125" t="s">
+      <c r="D103" s="149" t="s">
         <v>251</v>
       </c>
-      <c r="E103" s="125"/>
-      <c r="F103" s="125"/>
-      <c r="G103" s="125" t="s">
+      <c r="E103" s="149"/>
+      <c r="F103" s="149"/>
+      <c r="G103" s="149" t="s">
         <v>205</v>
       </c>
-      <c r="H103" s="125"/>
-      <c r="I103" s="125"/>
-      <c r="J103" s="125"/>
-      <c r="K103" s="125" t="s">
+      <c r="H103" s="149"/>
+      <c r="I103" s="149"/>
+      <c r="J103" s="149"/>
+      <c r="K103" s="149" t="s">
         <v>206</v>
       </c>
-      <c r="L103" s="125"/>
-      <c r="M103" s="125"/>
-      <c r="N103" s="125" t="s">
+      <c r="L103" s="149"/>
+      <c r="M103" s="149"/>
+      <c r="N103" s="149" t="s">
         <v>209</v>
       </c>
-      <c r="O103" s="125"/>
+      <c r="O103" s="149"/>
       <c r="P103" s="35" t="s">
         <v>283</v>
       </c>
       <c r="Q103" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="R103" s="124" t="s">
+      <c r="R103" s="148" t="s">
         <v>217</v>
       </c>
-      <c r="S103" s="124"/>
-      <c r="T103" s="124" t="s">
+      <c r="S103" s="148"/>
+      <c r="T103" s="148" t="s">
         <v>114</v>
       </c>
-      <c r="U103" s="124"/>
-      <c r="V103" s="125" t="s">
+      <c r="U103" s="148"/>
+      <c r="V103" s="149" t="s">
         <v>486</v>
       </c>
-      <c r="W103" s="125"/>
-      <c r="X103" s="125"/>
+      <c r="W103" s="149"/>
+      <c r="X103" s="149"/>
       <c r="Y103" s="35" t="s">
         <v>216</v>
       </c>
       <c r="Z103" s="35" t="s">
         <v>215</v>
       </c>
-      <c r="AA103" s="124" t="s">
+      <c r="AA103" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="AB103" s="124"/>
-      <c r="AC103" s="124"/>
-      <c r="AD103" s="124" t="s">
+      <c r="AB103" s="148"/>
+      <c r="AC103" s="148"/>
+      <c r="AD103" s="148" t="s">
         <v>224</v>
       </c>
-      <c r="AE103" s="124"/>
+      <c r="AE103" s="148"/>
       <c r="AF103" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="AG103" s="121"/>
-      <c r="AH103" s="121"/>
+      <c r="AG103" s="145"/>
+      <c r="AH103" s="145"/>
       <c r="AI103" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="AJ103" s="121"/>
-      <c r="AK103" s="121"/>
+      <c r="AJ103" s="145"/>
+      <c r="AK103" s="145"/>
       <c r="AL103" s="35" t="s">
         <v>129</v>
       </c>
@@ -9544,26 +9544,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="AS1:AS2"/>
-    <mergeCell ref="AT1:AT2"/>
-    <mergeCell ref="AU1:AU2"/>
-    <mergeCell ref="AV1:AV2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AM1:AM2"/>
-    <mergeCell ref="AN1:AN2"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AA1:AC1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:J1"/>
     <mergeCell ref="AG103:AH103"/>
     <mergeCell ref="AJ103:AK103"/>
     <mergeCell ref="B1:B2"/>
@@ -9580,6 +9560,26 @@
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="AS1:AS2"/>
+    <mergeCell ref="AT1:AT2"/>
+    <mergeCell ref="AU1:AU2"/>
+    <mergeCell ref="AV1:AV2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
+    <mergeCell ref="AN1:AN2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
hw: swap button 3 and 4, routing
</commit_message>
<xml_diff>
--- a/hw/pinout.xlsx
+++ b/hw/pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\RB3204-RBCX_hw\hw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robotarna\RB3204-RBCX_hw\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF86E83-3A4C-4E7F-9CD7-29BAAFBBF434}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1B09AA-B6C5-4156-9F8D-5313CFD9DA46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{08978B24-E42F-429B-A3F9-EF8F7AA6C2ED}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{08978B24-E42F-429B-A3F9-EF8F7AA6C2ED}"/>
   </bookViews>
   <sheets>
     <sheet name="koprocesor" sheetId="2" r:id="rId1"/>
@@ -2588,41 +2588,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2647,6 +2612,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2659,6 +2642,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3000,10 +3000,10 @@
   <dimension ref="A1:BQ114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AS3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BB4" sqref="BB4"/>
+      <selection pane="bottomRight" activeCell="AS83" sqref="AS83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3057,90 +3057,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:69" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="160" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="142" t="s">
+      <c r="B1" s="163" t="s">
         <v>254</v>
       </c>
       <c r="C1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="147" t="s">
+      <c r="D1" s="151" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="151"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="147" t="s">
+      <c r="E1" s="159"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="151" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="151"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="148"/>
-      <c r="K1" s="147" t="s">
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
+      <c r="J1" s="152"/>
+      <c r="K1" s="151" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="151"/>
-      <c r="M1" s="148"/>
-      <c r="N1" s="147" t="s">
+      <c r="L1" s="159"/>
+      <c r="M1" s="152"/>
+      <c r="N1" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="148"/>
-      <c r="P1" s="145" t="s">
+      <c r="O1" s="152"/>
+      <c r="P1" s="149" t="s">
         <v>94</v>
       </c>
-      <c r="Q1" s="145" t="s">
+      <c r="Q1" s="149" t="s">
         <v>95</v>
       </c>
-      <c r="R1" s="147" t="s">
+      <c r="R1" s="151" t="s">
         <v>114</v>
       </c>
-      <c r="S1" s="148"/>
-      <c r="T1" s="147" t="s">
+      <c r="S1" s="152"/>
+      <c r="T1" s="151" t="s">
         <v>113</v>
       </c>
-      <c r="U1" s="148"/>
-      <c r="V1" s="147" t="s">
+      <c r="U1" s="152"/>
+      <c r="V1" s="151" t="s">
         <v>115</v>
       </c>
-      <c r="W1" s="151"/>
-      <c r="X1" s="148"/>
-      <c r="Y1" s="145" t="s">
+      <c r="W1" s="159"/>
+      <c r="X1" s="152"/>
+      <c r="Y1" s="149" t="s">
         <v>296</v>
       </c>
-      <c r="Z1" s="145" t="s">
+      <c r="Z1" s="149" t="s">
         <v>297</v>
       </c>
-      <c r="AA1" s="147" t="s">
+      <c r="AA1" s="151" t="s">
         <v>122</v>
       </c>
-      <c r="AB1" s="151"/>
-      <c r="AC1" s="148"/>
-      <c r="AD1" s="147" t="s">
+      <c r="AB1" s="159"/>
+      <c r="AC1" s="152"/>
+      <c r="AD1" s="151" t="s">
         <v>123</v>
       </c>
-      <c r="AE1" s="148"/>
+      <c r="AE1" s="152"/>
       <c r="AF1" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="AG1" s="152" t="s">
+      <c r="AG1" s="153" t="s">
         <v>124</v>
       </c>
-      <c r="AH1" s="153"/>
-      <c r="AI1" s="145" t="s">
+      <c r="AH1" s="154"/>
+      <c r="AI1" s="149" t="s">
         <v>125</v>
       </c>
-      <c r="AJ1" s="152" t="s">
+      <c r="AJ1" s="153" t="s">
         <v>126</v>
       </c>
-      <c r="AK1" s="153"/>
-      <c r="AL1" s="145" t="s">
+      <c r="AK1" s="154"/>
+      <c r="AL1" s="149" t="s">
         <v>128</v>
       </c>
-      <c r="AM1" s="162" t="s">
+      <c r="AM1" s="155" t="s">
         <v>129</v>
       </c>
-      <c r="AN1" s="145" t="s">
+      <c r="AN1" s="149" t="s">
         <v>150</v>
       </c>
       <c r="AO1" s="7" t="s">
@@ -3155,28 +3155,28 @@
       <c r="AR1" s="49" t="s">
         <v>169</v>
       </c>
-      <c r="AS1" s="154" t="s">
+      <c r="AS1" s="141" t="s">
         <v>140</v>
       </c>
-      <c r="AT1" s="156" t="s">
+      <c r="AT1" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="AU1" s="158" t="s">
+      <c r="AU1" s="145" t="s">
         <v>181</v>
       </c>
-      <c r="AV1" s="164" t="s">
+      <c r="AV1" s="157" t="s">
         <v>182</v>
       </c>
       <c r="AW1" s="66" t="s">
         <v>468</v>
       </c>
-      <c r="AX1" s="160" t="s">
+      <c r="AX1" s="147" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="150"/>
-      <c r="B2" s="143"/>
+      <c r="A2" s="161"/>
+      <c r="B2" s="164"/>
       <c r="C2" s="67" t="s">
         <v>96</v>
       </c>
@@ -3216,8 +3216,8 @@
       <c r="O2" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="146"/>
-      <c r="Q2" s="146"/>
+      <c r="P2" s="150"/>
+      <c r="Q2" s="150"/>
       <c r="R2" s="68" t="s">
         <v>105</v>
       </c>
@@ -3239,8 +3239,8 @@
       <c r="X2" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="Y2" s="146"/>
-      <c r="Z2" s="146"/>
+      <c r="Y2" s="150"/>
+      <c r="Z2" s="150"/>
       <c r="AA2" s="68" t="s">
         <v>101</v>
       </c>
@@ -3263,26 +3263,26 @@
       <c r="AH2" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="AI2" s="146"/>
+      <c r="AI2" s="150"/>
       <c r="AJ2" s="68" t="s">
         <v>105</v>
       </c>
       <c r="AK2" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="AL2" s="146"/>
-      <c r="AM2" s="163"/>
-      <c r="AN2" s="146"/>
+      <c r="AL2" s="150"/>
+      <c r="AM2" s="156"/>
+      <c r="AN2" s="150"/>
       <c r="AO2" s="75"/>
       <c r="AP2" s="75"/>
       <c r="AQ2" s="75"/>
       <c r="AR2" s="75"/>
-      <c r="AS2" s="155"/>
-      <c r="AT2" s="157"/>
-      <c r="AU2" s="159"/>
-      <c r="AV2" s="165"/>
+      <c r="AS2" s="142"/>
+      <c r="AT2" s="144"/>
+      <c r="AU2" s="146"/>
+      <c r="AV2" s="158"/>
       <c r="AW2" s="76"/>
-      <c r="AX2" s="161"/>
+      <c r="AX2" s="148"/>
     </row>
     <row r="3" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A3" s="77">
@@ -3643,7 +3643,7 @@
         <v>250</v>
       </c>
       <c r="BD6" s="34" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="BE6" s="54" t="s">
         <v>198</v>
@@ -3895,7 +3895,7 @@
         <v>232</v>
       </c>
       <c r="BL8" s="34" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="BM8" s="34" t="s">
         <v>285</v>
@@ -6121,7 +6121,7 @@
         <v>32</v>
       </c>
       <c r="AV39" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="AW39" s="98">
         <v>2</v>
@@ -7437,7 +7437,7 @@
         <v>50</v>
       </c>
       <c r="AV59" s="113" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="AW59" s="118">
         <v>10</v>
@@ -10330,70 +10330,70 @@
       </c>
       <c r="B103"/>
       <c r="C103"/>
-      <c r="D103" s="144" t="s">
+      <c r="D103" s="165" t="s">
         <v>246</v>
       </c>
-      <c r="E103" s="144"/>
-      <c r="F103" s="144"/>
-      <c r="G103" s="144" t="s">
+      <c r="E103" s="165"/>
+      <c r="F103" s="165"/>
+      <c r="G103" s="165" t="s">
         <v>203</v>
       </c>
-      <c r="H103" s="144"/>
-      <c r="I103" s="144"/>
-      <c r="J103" s="144"/>
-      <c r="K103" s="144" t="s">
+      <c r="H103" s="165"/>
+      <c r="I103" s="165"/>
+      <c r="J103" s="165"/>
+      <c r="K103" s="165" t="s">
         <v>204</v>
       </c>
-      <c r="L103" s="144"/>
-      <c r="M103" s="144"/>
-      <c r="N103" s="144" t="s">
+      <c r="L103" s="165"/>
+      <c r="M103" s="165"/>
+      <c r="N103" s="165" t="s">
         <v>207</v>
       </c>
-      <c r="O103" s="144"/>
+      <c r="O103" s="165"/>
       <c r="P103" s="34" t="s">
         <v>208</v>
       </c>
       <c r="Q103" s="34" t="s">
         <v>276</v>
       </c>
-      <c r="R103" s="144" t="s">
+      <c r="R103" s="165" t="s">
         <v>471</v>
       </c>
-      <c r="S103" s="144"/>
-      <c r="T103" s="144" t="s">
+      <c r="S103" s="165"/>
+      <c r="T103" s="165" t="s">
         <v>470</v>
       </c>
-      <c r="U103" s="144"/>
-      <c r="V103" s="144" t="s">
+      <c r="U103" s="165"/>
+      <c r="V103" s="165" t="s">
         <v>469</v>
       </c>
-      <c r="W103" s="144"/>
-      <c r="X103" s="144"/>
+      <c r="W103" s="165"/>
+      <c r="X103" s="165"/>
       <c r="Y103" s="34" t="s">
         <v>213</v>
       </c>
       <c r="Z103" s="34" t="s">
         <v>483</v>
       </c>
-      <c r="AA103" s="144" t="s">
+      <c r="AA103" s="165" t="s">
         <v>214</v>
       </c>
-      <c r="AB103" s="144"/>
-      <c r="AC103" s="144"/>
-      <c r="AD103" s="144" t="s">
+      <c r="AB103" s="165"/>
+      <c r="AC103" s="165"/>
+      <c r="AD103" s="165" t="s">
         <v>220</v>
       </c>
-      <c r="AE103" s="144"/>
+      <c r="AE103" s="165"/>
       <c r="AF103" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="AG103" s="141"/>
-      <c r="AH103" s="141"/>
+      <c r="AG103" s="162"/>
+      <c r="AH103" s="162"/>
       <c r="AI103" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="AJ103" s="141"/>
-      <c r="AK103" s="141"/>
+      <c r="AJ103" s="162"/>
+      <c r="AK103" s="162"/>
       <c r="AL103" s="34" t="s">
         <v>128</v>
       </c>
@@ -10478,27 +10478,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="AS1:AS2"/>
-    <mergeCell ref="AT1:AT2"/>
-    <mergeCell ref="AU1:AU2"/>
-    <mergeCell ref="AX1:AX2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AM1:AM2"/>
-    <mergeCell ref="AN1:AN2"/>
-    <mergeCell ref="AV1:AV2"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AA1:AC1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:J1"/>
     <mergeCell ref="AG103:AH103"/>
     <mergeCell ref="AJ103:AK103"/>
     <mergeCell ref="B1:B2"/>
@@ -10515,6 +10494,27 @@
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AA1:AC1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="AS1:AS2"/>
+    <mergeCell ref="AT1:AT2"/>
+    <mergeCell ref="AU1:AU2"/>
+    <mergeCell ref="AX1:AX2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
+    <mergeCell ref="AN1:AN2"/>
+    <mergeCell ref="AV1:AV2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>